<commit_message>
Time period adaptation algorithm and visualization
</commit_message>
<xml_diff>
--- a/data/37-intersection map LIN S0 EV1 Solution.xlsx
+++ b/data/37-intersection map LIN S0 EV1 Solution.xlsx
@@ -534,7 +534,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
@@ -557,7 +557,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
@@ -580,7 +580,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="C6" t="n">
         <v>0</v>
@@ -603,7 +603,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="C7" t="n">
         <v>0</v>
@@ -747,7 +747,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="C13" t="n">
         <v>0</v>
@@ -770,7 +770,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="C14" t="n">
         <v>0</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="C15" t="n">
         <v>0</v>
@@ -1081,7 +1081,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="C27" t="n">
         <v>0</v>
@@ -1096,7 +1096,7 @@
         <v>0</v>
       </c>
       <c r="G27" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="H27" t="n">
         <v>0</v>
@@ -1108,7 +1108,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="C28" t="n">
         <v>0</v>
@@ -1131,7 +1131,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="C29" t="n">
         <v>0</v>
@@ -1202,7 +1202,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="C32" t="n">
         <v>0</v>
@@ -1225,7 +1225,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="C33" t="n">
         <v>0</v>
@@ -1271,7 +1271,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="C35" t="n">
         <v>0</v>
@@ -1294,7 +1294,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="C36" t="n">
         <v>0</v>
@@ -1439,7 +1439,7 @@
         <v>8</v>
       </c>
       <c r="C2" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
@@ -1456,7 +1456,7 @@
         <v>10</v>
       </c>
       <c r="C3" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D3" t="n">
         <v>0</v>
@@ -1473,7 +1473,7 @@
         <v>1</v>
       </c>
       <c r="C4" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D4" t="n">
         <v>0</v>
@@ -1490,7 +1490,7 @@
         <v>5</v>
       </c>
       <c r="C5" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D5" t="n">
         <v>0</v>
@@ -1524,7 +1524,7 @@
         <v>2</v>
       </c>
       <c r="C7" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D7" t="n">
         <v>0</v>
@@ -1541,7 +1541,7 @@
         <v>3</v>
       </c>
       <c r="C8" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D8" t="n">
         <v>0</v>
@@ -1558,7 +1558,7 @@
         <v>5</v>
       </c>
       <c r="C9" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D9" t="n">
         <v>0</v>
@@ -1575,7 +1575,7 @@
         <v>3</v>
       </c>
       <c r="C10" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D10" t="n">
         <v>0</v>
@@ -1592,7 +1592,7 @@
         <v>8</v>
       </c>
       <c r="C11" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D11" t="n">
         <v>0</v>
@@ -1609,7 +1609,7 @@
         <v>14</v>
       </c>
       <c r="C12" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D12" t="n">
         <v>0</v>
@@ -1626,7 +1626,7 @@
         <v>12</v>
       </c>
       <c r="C13" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D13" t="n">
         <v>0</v>
@@ -1643,7 +1643,7 @@
         <v>13</v>
       </c>
       <c r="C14" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D14" t="n">
         <v>0</v>
@@ -1660,7 +1660,7 @@
         <v>1</v>
       </c>
       <c r="C15" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D15" t="n">
         <v>0</v>
@@ -1694,7 +1694,7 @@
         <v>6</v>
       </c>
       <c r="C17" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D17" t="n">
         <v>0</v>
@@ -1728,7 +1728,7 @@
         <v>15</v>
       </c>
       <c r="C19" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D19" t="n">
         <v>0</v>
@@ -1762,7 +1762,7 @@
         <v>19</v>
       </c>
       <c r="C21" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D21" t="n">
         <v>0</v>
@@ -1779,7 +1779,7 @@
         <v>19</v>
       </c>
       <c r="C22" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D22" t="n">
         <v>0</v>
@@ -1796,7 +1796,7 @@
         <v>11</v>
       </c>
       <c r="C23" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D23" t="n">
         <v>0</v>
@@ -1813,7 +1813,7 @@
         <v>19</v>
       </c>
       <c r="C24" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D24" t="n">
         <v>0</v>
@@ -1847,7 +1847,7 @@
         <v>13</v>
       </c>
       <c r="C26" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D26" t="n">
         <v>0</v>
@@ -1864,7 +1864,7 @@
         <v>16</v>
       </c>
       <c r="C27" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D27" t="n">
         <v>0</v>
@@ -1881,7 +1881,7 @@
         <v>5</v>
       </c>
       <c r="C28" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D28" t="n">
         <v>0</v>
@@ -1898,7 +1898,7 @@
         <v>13</v>
       </c>
       <c r="C29" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D29" t="n">
         <v>0</v>
@@ -1915,7 +1915,7 @@
         <v>16</v>
       </c>
       <c r="C30" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D30" t="n">
         <v>0</v>
@@ -1932,7 +1932,7 @@
         <v>31</v>
       </c>
       <c r="C31" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D31" t="n">
         <v>0</v>
@@ -1966,7 +1966,7 @@
         <v>8</v>
       </c>
       <c r="C33" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D33" t="n">
         <v>0</v>
@@ -2017,7 +2017,7 @@
         <v>19</v>
       </c>
       <c r="C36" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D36" t="n">
         <v>0</v>
@@ -2034,7 +2034,7 @@
         <v>18</v>
       </c>
       <c r="C37" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D37" t="n">
         <v>0</v>
@@ -2051,7 +2051,7 @@
         <v>31</v>
       </c>
       <c r="C38" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D38" t="n">
         <v>0</v>
@@ -2068,7 +2068,7 @@
         <v>27</v>
       </c>
       <c r="C39" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D39" t="n">
         <v>0</v>
@@ -2085,7 +2085,7 @@
         <v>28</v>
       </c>
       <c r="C40" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D40" t="n">
         <v>0</v>
@@ -2136,7 +2136,7 @@
         <v>21</v>
       </c>
       <c r="C43" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D43" t="n">
         <v>0</v>
@@ -2153,7 +2153,7 @@
         <v>28</v>
       </c>
       <c r="C44" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D44" t="n">
         <v>0</v>
@@ -2187,7 +2187,7 @@
         <v>28</v>
       </c>
       <c r="C46" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D46" t="n">
         <v>0</v>
@@ -2204,7 +2204,7 @@
         <v>26</v>
       </c>
       <c r="C47" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D47" t="n">
         <v>0</v>
@@ -2289,7 +2289,7 @@
         <v>26</v>
       </c>
       <c r="C52" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D52" t="n">
         <v>0</v>
@@ -2323,7 +2323,7 @@
         <v>26</v>
       </c>
       <c r="C54" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D54" t="n">
         <v>0</v>
@@ -2340,7 +2340,7 @@
         <v>27</v>
       </c>
       <c r="C55" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D55" t="n">
         <v>0</v>
@@ -2357,7 +2357,7 @@
         <v>34</v>
       </c>
       <c r="C56" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D56" t="n">
         <v>0</v>
@@ -2391,7 +2391,7 @@
         <v>23</v>
       </c>
       <c r="C58" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D58" t="n">
         <v>0</v>
@@ -2408,7 +2408,7 @@
         <v>28</v>
       </c>
       <c r="C59" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D59" t="n">
         <v>0</v>
@@ -2425,7 +2425,7 @@
         <v>33</v>
       </c>
       <c r="C60" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D60" t="n">
         <v>0</v>
@@ -2442,7 +2442,7 @@
         <v>35</v>
       </c>
       <c r="C61" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D61" t="n">
         <v>0</v>
@@ -2476,7 +2476,7 @@
         <v>27</v>
       </c>
       <c r="C63" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D63" t="n">
         <v>0</v>
@@ -2493,7 +2493,7 @@
         <v>30</v>
       </c>
       <c r="C64" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D64" t="n">
         <v>0</v>
@@ -2544,7 +2544,7 @@
         <v>31</v>
       </c>
       <c r="C67" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D67" t="n">
         <v>0</v>
@@ -2578,7 +2578,7 @@
         <v>36</v>
       </c>
       <c r="C69" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D69" t="n">
         <v>0</v>
@@ -2595,7 +2595,7 @@
         <v>29</v>
       </c>
       <c r="C70" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D70" t="n">
         <v>0</v>
@@ -2612,7 +2612,7 @@
         <v>32</v>
       </c>
       <c r="C71" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D71" t="n">
         <v>0</v>
@@ -2646,7 +2646,7 @@
         <v>27</v>
       </c>
       <c r="C73" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D73" t="n">
         <v>0</v>
@@ -2663,7 +2663,7 @@
         <v>35</v>
       </c>
       <c r="C74" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D74" t="n">
         <v>0</v>
@@ -2680,7 +2680,7 @@
         <v>36</v>
       </c>
       <c r="C75" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D75" t="n">
         <v>0</v>
@@ -2731,7 +2731,7 @@
         <v>34</v>
       </c>
       <c r="C78" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D78" t="n">
         <v>0</v>
@@ -2816,7 +2816,7 @@
         <v>38</v>
       </c>
       <c r="C83" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D83" t="n">
         <v>0</v>
@@ -2850,7 +2850,7 @@
         <v>1</v>
       </c>
       <c r="C85" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D85" t="n">
         <v>0</v>
@@ -2901,7 +2901,7 @@
         <v>2</v>
       </c>
       <c r="C88" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D88" t="n">
         <v>0</v>
@@ -2918,7 +2918,7 @@
         <v>2</v>
       </c>
       <c r="C89" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D89" t="n">
         <v>0</v>
@@ -2935,7 +2935,7 @@
         <v>3</v>
       </c>
       <c r="C90" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D90" t="n">
         <v>0</v>
@@ -2952,7 +2952,7 @@
         <v>4</v>
       </c>
       <c r="C91" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D91" t="n">
         <v>0</v>
@@ -2969,7 +2969,7 @@
         <v>4</v>
       </c>
       <c r="C92" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D92" t="n">
         <v>0</v>
@@ -2986,7 +2986,7 @@
         <v>5</v>
       </c>
       <c r="C93" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D93" t="n">
         <v>0</v>
@@ -3003,7 +3003,7 @@
         <v>5</v>
       </c>
       <c r="C94" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D94" t="n">
         <v>0</v>
@@ -3020,7 +3020,7 @@
         <v>5</v>
       </c>
       <c r="C95" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D95" t="n">
         <v>0</v>
@@ -3037,7 +3037,7 @@
         <v>6</v>
       </c>
       <c r="C96" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D96" t="n">
         <v>0</v>
@@ -3054,7 +3054,7 @@
         <v>6</v>
       </c>
       <c r="C97" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D97" t="n">
         <v>0</v>
@@ -3071,7 +3071,7 @@
         <v>7</v>
       </c>
       <c r="C98" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D98" t="n">
         <v>0</v>
@@ -3088,7 +3088,7 @@
         <v>7</v>
       </c>
       <c r="C99" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D99" t="n">
         <v>0</v>
@@ -3105,7 +3105,7 @@
         <v>8</v>
       </c>
       <c r="C100" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D100" t="n">
         <v>0</v>
@@ -3122,7 +3122,7 @@
         <v>8</v>
       </c>
       <c r="C101" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D101" t="n">
         <v>0</v>
@@ -3139,7 +3139,7 @@
         <v>8</v>
       </c>
       <c r="C102" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D102" t="n">
         <v>0</v>
@@ -3156,7 +3156,7 @@
         <v>9</v>
       </c>
       <c r="C103" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D103" t="n">
         <v>0</v>
@@ -3173,7 +3173,7 @@
         <v>9</v>
       </c>
       <c r="C104" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D104" t="n">
         <v>0</v>
@@ -3258,7 +3258,7 @@
         <v>12</v>
       </c>
       <c r="C109" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D109" t="n">
         <v>0</v>
@@ -3292,7 +3292,7 @@
         <v>13</v>
       </c>
       <c r="C111" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D111" t="n">
         <v>0</v>
@@ -3326,7 +3326,7 @@
         <v>14</v>
       </c>
       <c r="C113" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D113" t="n">
         <v>0</v>
@@ -3343,7 +3343,7 @@
         <v>14</v>
       </c>
       <c r="C114" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D114" t="n">
         <v>0</v>
@@ -3360,7 +3360,7 @@
         <v>15</v>
       </c>
       <c r="C115" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D115" t="n">
         <v>0</v>
@@ -3377,7 +3377,7 @@
         <v>16</v>
       </c>
       <c r="C116" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D116" t="n">
         <v>0</v>
@@ -3394,7 +3394,7 @@
         <v>16</v>
       </c>
       <c r="C117" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D117" t="n">
         <v>0</v>
@@ -3411,7 +3411,7 @@
         <v>16</v>
       </c>
       <c r="C118" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D118" t="n">
         <v>0</v>
@@ -3428,7 +3428,7 @@
         <v>16</v>
       </c>
       <c r="C119" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D119" t="n">
         <v>0</v>
@@ -3462,7 +3462,7 @@
         <v>17</v>
       </c>
       <c r="C121" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D121" t="n">
         <v>0</v>
@@ -3479,7 +3479,7 @@
         <v>18</v>
       </c>
       <c r="C122" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D122" t="n">
         <v>0</v>
@@ -3496,7 +3496,7 @@
         <v>18</v>
       </c>
       <c r="C123" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D123" t="n">
         <v>0</v>
@@ -3530,7 +3530,7 @@
         <v>19</v>
       </c>
       <c r="C125" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D125" t="n">
         <v>0</v>
@@ -3564,7 +3564,7 @@
         <v>19</v>
       </c>
       <c r="C127" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D127" t="n">
         <v>0</v>
@@ -3581,7 +3581,7 @@
         <v>20</v>
       </c>
       <c r="C128" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D128" t="n">
         <v>0</v>
@@ -3598,7 +3598,7 @@
         <v>21</v>
       </c>
       <c r="C129" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D129" t="n">
         <v>0</v>
@@ -3615,7 +3615,7 @@
         <v>22</v>
       </c>
       <c r="C130" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D130" t="n">
         <v>0</v>
@@ -3632,7 +3632,7 @@
         <v>23</v>
       </c>
       <c r="C131" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D131" t="n">
         <v>0</v>
@@ -3734,7 +3734,7 @@
         <v>25</v>
       </c>
       <c r="C137" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D137" t="n">
         <v>0</v>
@@ -3751,7 +3751,7 @@
         <v>25</v>
       </c>
       <c r="C138" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D138" t="n">
         <v>0</v>
@@ -3768,7 +3768,7 @@
         <v>25</v>
       </c>
       <c r="C139" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D139" t="n">
         <v>0</v>
@@ -3802,7 +3802,7 @@
         <v>27</v>
       </c>
       <c r="C141" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D141" t="n">
         <v>0</v>
@@ -3819,7 +3819,7 @@
         <v>27</v>
       </c>
       <c r="C142" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D142" t="n">
         <v>0</v>
@@ -3836,7 +3836,7 @@
         <v>27</v>
       </c>
       <c r="C143" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D143" t="n">
         <v>0</v>
@@ -3853,7 +3853,7 @@
         <v>27</v>
       </c>
       <c r="C144" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D144" t="n">
         <v>0</v>
@@ -3870,7 +3870,7 @@
         <v>29</v>
       </c>
       <c r="C145" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D145" t="n">
         <v>0</v>
@@ -3887,7 +3887,7 @@
         <v>29</v>
       </c>
       <c r="C146" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D146" t="n">
         <v>0</v>
@@ -3955,7 +3955,7 @@
         <v>30</v>
       </c>
       <c r="C150" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D150" t="n">
         <v>0</v>
@@ -3972,7 +3972,7 @@
         <v>30</v>
       </c>
       <c r="C151" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D151" t="n">
         <v>0</v>
@@ -3989,7 +3989,7 @@
         <v>31</v>
       </c>
       <c r="C152" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D152" t="n">
         <v>0</v>
@@ -4057,7 +4057,7 @@
         <v>34</v>
       </c>
       <c r="C156" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D156" t="n">
         <v>0</v>
@@ -4074,7 +4074,7 @@
         <v>34</v>
       </c>
       <c r="C157" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D157" t="n">
         <v>0</v>
@@ -4091,7 +4091,7 @@
         <v>35</v>
       </c>
       <c r="C158" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D158" t="n">
         <v>0</v>
@@ -4142,7 +4142,7 @@
         <v>37</v>
       </c>
       <c r="C161" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D161" t="n">
         <v>0</v>
@@ -4193,7 +4193,7 @@
         <v>38</v>
       </c>
       <c r="C164" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D164" t="n">
         <v>0</v>
@@ -4210,7 +4210,7 @@
         <v>38</v>
       </c>
       <c r="C165" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D165" t="n">
         <v>0</v>

</xml_diff>